<commit_message>
В папку "Models" добавлены папки: 1)"Cart", включающая класс IndexDTO.cs; 2)"Orders", включающая классы OrderProductDTO.cs, OrderRegistrationDTO.cs, OrdersDataDTO.cs; 3)"Payment", включающая класс IndexDTO.cs; 4)"PersonalData", включающая класс PersonalAreaDTO.cs; 5)"ProductsData", включающая классы PageCatalogDTO.cs, ProductDetailsDTO.cs, ProductsCatalogDTO.cs; 6)"Reviews", включающая класс IndexDTO.cs
</commit_message>
<xml_diff>
--- a/src/МакетMyShop.xlsx
+++ b/src/МакетMyShop.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Лёлька\source\repos\MyShop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\MySuperShop\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4695" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4695" firstSheet="14" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Стартовая страница" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="Оформить заказ" sheetId="17" r:id="rId17"/>
     <sheet name="Перейти к оплате" sheetId="18" r:id="rId18"/>
     <sheet name="Оплатить" sheetId="19" r:id="rId19"/>
+    <sheet name="Лист1" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="164">
   <si>
     <t>Дата рождения</t>
   </si>
@@ -639,6 +640,30 @@
   </si>
   <si>
     <t>Товар добавлен в корзину!</t>
+  </si>
+  <si>
+    <t>Текущий заказ</t>
+  </si>
+  <si>
+    <t>Каталог товаров?</t>
+  </si>
+  <si>
+    <t>Любая страница  из каталога</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Подробнее о товаре </t>
+  </si>
+  <si>
+    <t>Корзина</t>
+  </si>
+  <si>
+    <t>Оплата</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Артикул товара</t>
   </si>
 </sst>
 </file>
@@ -762,12 +787,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="20">
@@ -1004,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1244,6 +1275,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -2280,7 +2312,7 @@
   </sheetPr>
   <dimension ref="B2:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -2684,8 +2716,8 @@
   </sheetPr>
   <dimension ref="B2:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I5"/>
+    <sheetView topLeftCell="A15" zoomScale="84" workbookViewId="0">
+      <selection activeCell="A35" sqref="A28:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3459,8 +3491,8 @@
   </sheetPr>
   <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I2"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3857,7 +3889,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:H9"/>
+      <selection activeCell="C6" sqref="C6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4208,7 +4240,7 @@
   </sheetPr>
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -4593,8 +4625,8 @@
   </sheetPr>
   <dimension ref="B2:Q36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:H11"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5015,8 +5047,8 @@
   </sheetPr>
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5734,7 +5766,7 @@
   </sheetPr>
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E19" sqref="E19:F19"/>
     </sheetView>
   </sheetViews>
@@ -6086,6 +6118,81 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E19:F19"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="103"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="103"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="103" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="103"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="103" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="103"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="103" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="103"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="103" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="103" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6787,9 +6894,9 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="B2:I34"/>
+  <dimension ref="B2:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -7136,7 +7243,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -7146,7 +7253,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -7155,6 +7262,11 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>162</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7886,22 +7998,22 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:P32"/>
+  <dimension ref="B2:Q32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -7910,52 +8022,56 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="36"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="40"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J3" s="9"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="40"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="73"/>
       <c r="G4" s="73"/>
       <c r="H4" s="73"/>
       <c r="I4" s="73"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="40"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J4" s="73"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="40"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="40"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J5" s="6"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="40"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -7965,10 +8081,11 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
-      <c r="P6" s="29"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K6" s="6"/>
+      <c r="L6" s="7"/>
+      <c r="Q6" s="29"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -7978,9 +8095,10 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K7" s="6"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="55" t="s">
         <v>144</v>
       </c>
@@ -7992,9 +8110,10 @@
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
       <c r="J8" s="56"/>
-      <c r="K8" s="57"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K8" s="56"/>
+      <c r="L8" s="57"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -8004,9 +8123,10 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K9" s="6"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -8016,9 +8136,10 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>147</v>
       </c>
@@ -8028,92 +8149,105 @@
       <c r="D11" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="I11" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="J11" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="I12" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="J12" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="I13" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="29" t="s">
+      <c r="J13" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="I14" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="J14" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="I15" s="29" t="s">
+      <c r="H15" s="6"/>
+      <c r="J15" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -8123,9 +8257,10 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -8135,9 +8270,10 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="7"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="6"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>147</v>
       </c>
@@ -8147,91 +8283,104 @@
       <c r="D18" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="29" t="s">
+      <c r="I18" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I18" s="29" t="s">
+      <c r="J18" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="6"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="I19" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I19" s="29" t="s">
+      <c r="J19" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="6"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="I20" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="29" t="s">
+      <c r="J20" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="6"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="I21" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="J21" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="6"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29" t="s">
+      <c r="H22" s="6"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="6"/>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -8241,9 +8390,10 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="6"/>
+      <c r="L23" s="7"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -8253,9 +8403,10 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="6"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>147</v>
       </c>
@@ -8265,93 +8416,106 @@
       <c r="D25" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="I25" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="J25" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="6"/>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H26" s="29" t="s">
+      <c r="I26" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I26" s="29" t="s">
+      <c r="J26" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="6"/>
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="I27" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I27" s="29" t="s">
+      <c r="J27" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="6"/>
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H28" s="29" t="s">
+      <c r="I28" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="I28" s="29" t="s">
+      <c r="J28" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="6"/>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29" t="s">
+      <c r="H29" s="6"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="6"/>
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -8361,9 +8525,10 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="6"/>
+      <c r="L30" s="7"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -8373,9 +8538,10 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="7"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="6"/>
+      <c r="L31" s="7"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -8385,12 +8551,13 @@
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
-      <c r="K32" s="10"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="B8:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8404,7 +8571,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>